<commit_message>
Idaho file udpates 092020
Idaho file udpates 092020.  Cleaning code.
</commit_message>
<xml_diff>
--- a/Idaho/WaterAllocation/ID_Allocatoin Schema Mapping_WaDEQA.xlsx
+++ b/Idaho/WaterAllocation/ID_Allocatoin Schema Mapping_WaDEQA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Idaho\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA438C-32EE-4407-BDF2-4D68639540E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FF721E-4B9C-4771-B49D-65ED386E285E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="1440" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes and Reminders" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="332">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -980,22 +980,6 @@
     <t>Status</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Status'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If blank, = "Unknown'</t>
-    </r>
-  </si>
-  <si>
     <t>*We need Idaho to confirm how to treat this. For Idaho, CFS is specific to WR, but the volume is by use site.</t>
   </si>
   <si>
@@ -1133,6 +1117,30 @@
   </si>
   <si>
     <t>Author: Ryan James</t>
+  </si>
+  <si>
+    <t>Links to Data</t>
+  </si>
+  <si>
+    <t>Point of Diversion (POD): (download spreadsheet)</t>
+  </si>
+  <si>
+    <t>https://data-idwr.opendata.arcgis.com/datasets/water-right-pods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place of Use (PoU): Water Right (download the Zipped Files). See metadata in the View. Open WaterRightPOUs.dbf into Excel/load it into pandas Python </t>
+  </si>
+  <si>
+    <t>https://data-idwr.opendata.arcgis.com/pages/gis-data#WaterRights</t>
+  </si>
+  <si>
+    <t>Seasons of Use (SoU):  contains begin and end data of water use, split into water basins</t>
+  </si>
+  <si>
+    <t>https://data-idwr.opendata.arcgis.com/datasets/282b354f586144e596e309e09dd16a00_2</t>
+  </si>
+  <si>
+    <t>If blank, = "Unknown'</t>
   </si>
 </sst>
 </file>
@@ -1877,7 +1885,7 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2170,6 +2178,30 @@
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2537,17 +2569,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72E64E2-72A8-46D3-9648-0C1B18AE26B8}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -2572,27 +2604,62 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3807,8 +3874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC5F405-0A84-4CAE-BAB0-9DF044EAE9B9}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4530,7 +4597,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>170</v>
@@ -4562,7 +4629,7 @@
         <v>41</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>170</v>
@@ -4656,7 +4723,7 @@
         <v>41</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F17" s="22" t="s">
         <v>170</v>
@@ -4691,7 +4758,7 @@
         <v>172</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G18" s="25" t="s">
         <v>41</v>
@@ -4703,7 +4770,7 @@
         <v>3703994</v>
       </c>
       <c r="J18" s="28" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -4847,8 +4914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5169,7 +5236,7 @@
         <v>41</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F11" s="36" t="s">
         <v>41</v>
@@ -5233,7 +5300,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F13" s="65"/>
       <c r="G13" s="66" t="s">
@@ -5266,10 +5333,10 @@
         <v>41</v>
       </c>
       <c r="F14" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="G14" s="55" t="s">
         <v>286</v>
-      </c>
-      <c r="G14" s="55" t="s">
-        <v>287</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>41</v>
@@ -5283,7 +5350,7 @@
     </row>
     <row r="15" spans="1:10" s="82" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="82" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B15" s="83" t="s">
         <v>36</v>
@@ -5390,23 +5457,19 @@
       <c r="D18" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="G18" s="94" t="s">
-        <v>300</v>
-      </c>
+      <c r="E18" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="48"/>
+      <c r="G18" s="94"/>
       <c r="H18" s="83" t="s">
         <v>41</v>
       </c>
       <c r="I18" s="87" t="s">
+        <v>319</v>
+      </c>
+      <c r="J18" s="31" t="s">
         <v>320</v>
-      </c>
-      <c r="J18" s="31" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -5507,7 +5570,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>36</v>
@@ -5537,27 +5600,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="36" t="s">
-        <v>284</v>
-      </c>
-      <c r="F23" s="48" t="s">
+      <c r="E23" s="101" t="s">
+        <v>331</v>
+      </c>
+      <c r="F23" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="G23" s="30" t="s">
-        <v>283</v>
+      <c r="G23" s="103" t="s">
+        <v>299</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>41</v>
@@ -5667,7 +5730,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>36</v>
@@ -5691,7 +5754,7 @@
         <v>41</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J27" s="60" t="s">
         <v>41</v>
@@ -5726,7 +5789,7 @@
         <v>44196</v>
       </c>
       <c r="J28" s="74" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -5743,10 +5806,10 @@
         <v>41</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F29" s="36" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G29" s="37" t="s">
         <v>41</v>
@@ -5758,44 +5821,44 @@
         <v>43831</v>
       </c>
       <c r="J29" s="74" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I30" s="13" t="s">
+      <c r="E30" s="101" t="s">
+        <v>331</v>
+      </c>
+      <c r="F30" s="102" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="104" t="s">
+        <v>283</v>
+      </c>
+      <c r="H30" s="99" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="J30" s="60" t="s">
+      <c r="J30" s="106" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>37</v>
@@ -5810,10 +5873,10 @@
         <v>275</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G31" s="73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H31" s="59" t="s">
         <v>41</v>
@@ -5923,7 +5986,7 @@
     </row>
     <row r="35" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="82" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B35" s="83" t="s">
         <v>36</v>
@@ -5935,7 +5998,7 @@
         <v>41</v>
       </c>
       <c r="E35" s="97" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F35" s="47" t="s">
         <v>41</v>
@@ -6044,7 +6107,7 @@
         <v>41</v>
       </c>
       <c r="J38" s="51" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -6177,7 +6240,7 @@
     </row>
     <row r="43" spans="1:10" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="82" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B43" s="83" t="s">
         <v>115</v>
@@ -6204,12 +6267,12 @@
         <v>143</v>
       </c>
       <c r="J43" s="98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>18</v>
@@ -6297,18 +6360,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="77" t="s">
         <v>304</v>
       </c>
-      <c r="B2" s="77" t="s">
-        <v>305</v>
-      </c>
       <c r="C2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -6324,10 +6387,10 @@
         <v>89</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -6383,10 +6446,10 @@
         <v>91</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6426,10 +6489,10 @@
         <v>90</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -6437,10 +6500,10 @@
         <v>102</v>
       </c>
       <c r="B17" s="78" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -6472,10 +6535,10 @@
         <v>153</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -6507,10 +6570,10 @@
         <v>86</v>
       </c>
       <c r="B25" s="78" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -6526,7 +6589,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="78" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -6587,10 +6650,10 @@
         <v>85</v>
       </c>
       <c r="B35" s="78" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>